<commit_message>
average, count, autosum, autofill
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supev\Documents\EOQ\udemy\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519E86A-745D-4334-ADBF-015375D72238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B9FA2D-394F-4FB2-BD53-2972E66AB11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29E645FF-D4B7-43DA-9CB1-4EA40314491C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,7 +115,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,13 +453,14 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -521,11 +525,11 @@
         <v>100</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
         <v>350</v>
       </c>
       <c r="F5">
-        <f>E5/$E$9</f>
+        <f t="shared" ref="F5:F9" si="1">E5/$E$9</f>
         <v>6.8292682926829273E-2</v>
       </c>
     </row>
@@ -543,11 +547,11 @@
         <v>175</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>525</v>
       </c>
       <c r="F6">
-        <f>E6/$E$9</f>
+        <f t="shared" si="1"/>
         <v>0.1024390243902439</v>
       </c>
     </row>
@@ -565,11 +569,11 @@
         <v>350</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>925</v>
       </c>
       <c r="F7">
-        <f>E7/$E$9</f>
+        <f t="shared" si="1"/>
         <v>0.18048780487804877</v>
       </c>
     </row>
@@ -587,11 +591,11 @@
         <v>125</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>325</v>
       </c>
       <c r="F8">
-        <f>E8/$E$9</f>
+        <f t="shared" si="1"/>
         <v>6.3414634146341464E-2</v>
       </c>
     </row>
@@ -604,19 +608,19 @@
         <v>1675</v>
       </c>
       <c r="C9">
-        <f>SUM(C4:C8)</f>
+        <f t="shared" ref="C9:E9" si="2">SUM(C4:C8)</f>
         <v>1700</v>
       </c>
       <c r="D9">
-        <f>SUM(D4:D8)</f>
+        <f t="shared" si="2"/>
         <v>1750</v>
       </c>
       <c r="E9">
-        <f>SUM(E4:E8)</f>
+        <f t="shared" si="2"/>
         <v>5125</v>
       </c>
       <c r="F9">
-        <f>E9/$E$9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -651,15 +655,15 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:E12" si="0">MAX(C4:C8)</f>
+        <f t="shared" ref="C12:E12" si="3">MAX(C4:C8)</f>
         <v>1000</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
     </row>
@@ -667,6 +671,43 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <f>AVERAGE(B4:B8)</f>
+        <v>335</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C4:C8)</f>
+        <v>340</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D4:D8)</f>
+        <v>350</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E4:E8)</f>
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B4:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f>COUNT(C4:C8)</f>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f>COUNT(D4:D8)</f>
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f>COUNT(E4:E8)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" s="1"/>
@@ -674,5 +715,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B10:D14 B3:F3 B5:D8 B4:D4" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>